<commit_message>
Update dataset and add some code
</commit_message>
<xml_diff>
--- a/data/Station_Records.xlsx
+++ b/data/Station_Records.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smu-my.sharepoint.com/personal/serena_lew_2022_mitb_smu_edu_sg/Documents/Term 4 Jan-Apr 2024/ISSS 608  Visual Analytics and Applications/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smu-my.sharepoint.com/personal/serena_lew_2022_mitb_smu_edu_sg/Documents/Term 4 Jan-Apr 2024/ISSS 608  Visual Analytics and Applications/Project/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_0A53E398CF74926C75423D67C360A31940F1E52E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A513328-429B-43DE-BE1E-2D0CC77ED097}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="11_0A53E398CF74926C75423D67C360A31940F1E52E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94104154-B174-4BE2-8518-666F11E73CB9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -465,27 +464,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">East Coast
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Parkway</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -913,17 +891,6 @@
         <family val="2"/>
       </rPr>
       <t>Jan 2014-Nov 2015</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Admiralty (West)</t>
     </r>
   </si>
   <si>
@@ -1039,17 +1006,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Somerset</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Punggol</t>
     </r>
   </si>
@@ -1148,17 +1104,6 @@
         <family val="2"/>
       </rPr>
       <t>Buona Vista</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Pasir Ris Central</t>
     </r>
   </si>
   <si>
@@ -1551,6 +1496,18 @@
   </si>
   <si>
     <t>Station Name</t>
+  </si>
+  <si>
+    <t>East Coast Parkway</t>
+  </si>
+  <si>
+    <t>Pasir Ris (Central)</t>
+  </si>
+  <si>
+    <t>Admiralty West</t>
+  </si>
+  <si>
+    <t>Somerset (Road)</t>
   </si>
 </sst>
 </file>
@@ -1585,7 +1542,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1600,6 +1557,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDD9C3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1736,7 +1699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1796,6 +1759,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2104,12 +2070,13 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.69921875" customWidth="1"/>
+    <col min="1" max="1" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.69921875" customWidth="1"/>
     <col min="3" max="3" width="10.3984375" customWidth="1"/>
     <col min="4" max="4" width="12.69921875" customWidth="1"/>
     <col min="5" max="10" width="19.796875" customWidth="1"/>
@@ -2117,16 +2084,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="42.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>0</v>
@@ -2148,11 +2115,11 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C2" s="5">
         <v>1.3524</v>
@@ -2180,11 +2147,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C3" s="5">
         <v>1.3857999999999999</v>
@@ -2212,11 +2179,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C4" s="5">
         <v>1.3677999999999999</v>
@@ -2244,11 +2211,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C5" s="5">
         <v>1.4166000000000001</v>
@@ -2276,11 +2243,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C6" s="5">
         <v>1.3399000000000001</v>
@@ -2308,11 +2275,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C7" s="5">
         <v>1.3454999999999999</v>
@@ -2340,11 +2307,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="20" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C8" s="5">
         <v>1.3764000000000001</v>
@@ -2372,11 +2339,11 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C9" s="5">
         <v>1.3337000000000001</v>
@@ -2404,11 +2371,11 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C10" s="5">
         <v>1.4439</v>
@@ -2436,11 +2403,11 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="20" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C11" s="5">
         <v>1.25</v>
@@ -2468,11 +2435,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C12" s="5">
         <v>1.4252</v>
@@ -2500,11 +2467,11 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C13" s="5">
         <v>1.3302</v>
@@ -2532,11 +2499,11 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C14" s="5">
         <v>1.1890000000000001</v>
@@ -2564,11 +2531,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C15" s="5">
         <v>1.4168000000000001</v>
@@ -2596,11 +2563,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>41</v>
+      <c r="A16" s="20" t="s">
+        <v>185</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C16" s="5">
         <v>1.3133999999999999</v>
@@ -2609,30 +2576,30 @@
         <v>103.9619</v>
       </c>
       <c r="E16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="B17" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C17" s="5">
         <v>1.2799</v>
@@ -2641,30 +2608,30 @@
         <v>103.8703</v>
       </c>
       <c r="E17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="B18" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C18" s="5">
         <v>1.3106</v>
@@ -2673,30 +2640,30 @@
         <v>103.8365</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="B19" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C19" s="5">
         <v>1.2938000000000001</v>
@@ -2705,30 +2672,30 @@
         <v>103.61839999999999</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="B20" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C20" s="5">
         <v>1.2809999999999999</v>
@@ -2756,11 +2723,11 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>50</v>
+      <c r="A21" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C21" s="5">
         <v>1.2542</v>
@@ -2769,30 +2736,30 @@
         <v>103.6741</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="B22" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C22" s="7">
         <v>1.3729</v>
@@ -2801,30 +2768,30 @@
         <v>103.72239999999999</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>53</v>
+      <c r="A23" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C23" s="5">
         <v>1.4173</v>
@@ -2833,30 +2800,30 @@
         <v>103.8249</v>
       </c>
       <c r="E23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="G23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C24" s="5">
         <v>1.3416999999999999</v>
@@ -2877,10 +2844,10 @@
     </row>
     <row r="25" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C25" s="7">
         <v>1.3701000000000001</v>
@@ -2901,10 +2868,10 @@
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C26" s="5">
         <v>1.3863000000000001</v>
@@ -2925,10 +2892,10 @@
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C27" s="5">
         <v>1.2745</v>
@@ -2937,10 +2904,10 @@
         <v>103.828</v>
       </c>
       <c r="E27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
@@ -2949,10 +2916,10 @@
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C28" s="5">
         <v>1.3081</v>
@@ -2973,10 +2940,10 @@
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C29" s="5">
         <v>1.3329</v>
@@ -2997,10 +2964,10 @@
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C30" s="5">
         <v>1.3382000000000001</v>
@@ -3021,10 +2988,10 @@
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C31" s="5">
         <v>1.3262</v>
@@ -3033,10 +3000,10 @@
         <v>103.7354</v>
       </c>
       <c r="E31" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
@@ -3045,10 +3012,10 @@
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C32" s="5">
         <v>1.4036</v>
@@ -3069,10 +3036,10 @@
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C33" s="5">
         <v>1.3415999999999999</v>
@@ -3081,10 +3048,10 @@
         <v>103.81059999999999</v>
       </c>
       <c r="E33" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
@@ -3093,10 +3060,10 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C34" s="5">
         <v>1.3836999999999999</v>
@@ -3105,10 +3072,10 @@
         <v>103.886</v>
       </c>
       <c r="E34" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
@@ -3117,10 +3084,10 @@
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C35" s="5">
         <v>1.3274999999999999</v>
@@ -3129,10 +3096,10 @@
         <v>103.7042</v>
       </c>
       <c r="E35" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="15"/>
@@ -3141,10 +3108,10 @@
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C36" s="5">
         <v>1.3824000000000001</v>
@@ -3165,10 +3132,10 @@
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C37" s="5">
         <v>1.4387000000000001</v>
@@ -3189,10 +3156,10 @@
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C38" s="5">
         <v>1.274</v>
@@ -3201,10 +3168,10 @@
         <v>103.84820000000001</v>
       </c>
       <c r="E38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="G38" s="14"/>
       <c r="H38" s="15"/>
@@ -3213,10 +3180,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C39" s="5">
         <v>1.4581999999999999</v>
@@ -3225,10 +3192,10 @@
         <v>103.7953</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G39" s="14"/>
       <c r="H39" s="15"/>
@@ -3237,10 +3204,10 @@
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C40" s="5">
         <v>1.2937000000000001</v>
@@ -3261,10 +3228,10 @@
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C41" s="5">
         <v>1.3069999999999999</v>
@@ -3285,10 +3252,10 @@
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C42" s="5">
         <v>1.3277000000000001</v>
@@ -3297,7 +3264,7 @@
         <v>103.9203</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>17</v>
@@ -3309,10 +3276,10 @@
     </row>
     <row r="43" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C43" s="5">
         <v>1.37</v>
@@ -3321,7 +3288,7 @@
         <v>103.80500000000001</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>17</v>
@@ -3333,10 +3300,10 @@
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C44" s="5">
         <v>1.2923</v>
@@ -3357,10 +3324,10 @@
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>93</v>
+        <v>188</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C45" s="5">
         <v>1.3004</v>
@@ -3369,7 +3336,7 @@
         <v>103.8372</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>17</v>
@@ -3381,10 +3348,10 @@
     </row>
     <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C46" s="5">
         <v>1.4029</v>
@@ -3393,7 +3360,7 @@
         <v>103.9092</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>17</v>
@@ -3405,10 +3372,10 @@
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C47" s="5">
         <v>1.3247</v>
@@ -3429,10 +3396,10 @@
     </row>
     <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C48" s="5">
         <v>1.3436999999999999</v>
@@ -3441,7 +3408,7 @@
         <v>103.9444</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>17</v>
@@ -3453,10 +3420,10 @@
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C49" s="5">
         <v>1.3414999999999999</v>
@@ -3477,10 +3444,10 @@
     </row>
     <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C50" s="5">
         <v>1.3199000000000001</v>
@@ -3501,10 +3468,10 @@
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C51" s="5">
         <v>1.3190999999999999</v>
@@ -3525,10 +3492,10 @@
     </row>
     <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C52" s="5">
         <v>1.4300999999999999</v>
@@ -3537,10 +3504,10 @@
         <v>103.8308</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="15"/>
@@ -3549,10 +3516,10 @@
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C53" s="5">
         <v>1.2841</v>
@@ -3573,10 +3540,10 @@
     </row>
     <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>104</v>
+        <v>186</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C54" s="5">
         <v>1.3678999999999999</v>
@@ -3597,10 +3564,10 @@
     </row>
     <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C55" s="5">
         <v>1.3505</v>
@@ -3609,10 +3576,10 @@
         <v>103.71339999999999</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G55" s="14"/>
       <c r="H55" s="15"/>
@@ -3621,10 +3588,10 @@
     </row>
     <row r="56" spans="1:10" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C56" s="5">
         <v>1.3746</v>
@@ -3645,10 +3612,10 @@
     </row>
     <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C57" s="5">
         <v>1.3606</v>
@@ -3657,10 +3624,10 @@
         <v>103.86969999999999</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="12"/>
@@ -3669,10 +3636,10 @@
     </row>
     <row r="58" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C58" s="5">
         <v>1.4384999999999999</v>
@@ -3693,10 +3660,10 @@
     </row>
     <row r="59" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C59" s="5">
         <v>1.3065</v>
@@ -3705,7 +3672,7 @@
         <v>103.91070000000001</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>17</v>
@@ -3717,10 +3684,10 @@
     </row>
     <row r="60" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C60" s="5">
         <v>1.3818999999999999</v>
@@ -3729,7 +3696,7 @@
         <v>103.73860000000001</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>17</v>
@@ -3741,10 +3708,10 @@
     </row>
     <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C61" s="5">
         <v>1.2994000000000001</v>
@@ -3753,7 +3720,7 @@
         <v>103.84610000000001</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>17</v>
@@ -3765,10 +3732,10 @@
     </row>
     <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C62" s="5">
         <v>1.3010999999999999</v>
@@ -3777,7 +3744,7 @@
         <v>103.86660000000001</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>17</v>
@@ -3789,10 +3756,10 @@
     </row>
     <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C63" s="5">
         <v>1.3087</v>
@@ -3801,7 +3768,7 @@
         <v>103.818</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>17</v>
@@ -3813,10 +3780,10 @@
     </row>
     <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C64" s="5">
         <v>1.3213999999999999</v>
@@ -3825,7 +3792,7 @@
         <v>103.85769999999999</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>17</v>

</xml_diff>